<commit_message>
Finalised the merging of USYD
</commit_message>
<xml_diff>
--- a/test_USYD.xlsx
+++ b/test_USYD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westernsydneyedu.sharepoint.com/sites/ScholarshipsOperationsGroup/Shared Documents/Git/Scholarships/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1776" documentId="11_02A169CE2EF2BE07F727D8CF02F0AE323586B34E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97F3BFFF-225F-450D-A3EC-1801252DB444}"/>
+  <xr:revisionPtr revIDLastSave="1821" documentId="11_02A169CE2EF2BE07F727D8CF02F0AE323586B34E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D88E6EDD-09C8-4D3E-9EEA-7EA27C111751}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,11 +650,6 @@
 • Provide statement</t>
   </si>
   <si>
-    <t>• Low-socioeconomic background
-• Piano student
-• Provide statement</t>
-  </si>
-  <si>
     <t>• School of Business programs
 • Academic merit (ATAR)
 • Provide statement</t>
@@ -1918,6 +1913,11 @@
     <t>• Bachelor of Pharmacy and Management (Honours)  
 • Academic merit (ATAR) 
 • Rural or Regional - Preference</t>
+  </si>
+  <si>
+    <t>• Low SES
+• Piano student
+• Provide statement</t>
   </si>
 </sst>
 </file>
@@ -2033,10 +2033,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2326,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,7 +2377,7 @@
         <v>Alan Hyland Scholarship for Instrumental Studies</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -2471,7 +2467,7 @@
         <v>Alison Burrell Bequest</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -2561,7 +2557,7 @@
         <v>Anthony and Sharon Lee Foundation Jazz Scholarship</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>69</v>
@@ -2591,7 +2587,7 @@
         <v>Anthony Strachan Scholarship</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -2603,7 +2599,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
@@ -2621,7 +2617,7 @@
         <v>Belinda Frances Hughes Piano Scholarship</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2651,7 +2647,7 @@
         <v>Belinda Frances Hughes Violin Scholarship</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -2681,7 +2677,7 @@
         <v>The Bessie Cook Piano Award</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -2711,7 +2707,7 @@
         <v>Board of Governors' Scholarship</v>
       </c>
       <c r="C13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -2723,7 +2719,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H13" t="s">
         <v>13</v>
@@ -2771,7 +2767,7 @@
         <v>Bruce A Pontin Memorial Scholarship</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -2921,7 +2917,7 @@
         <v>Cary James and Anne Witheford Back of Orchestra Scholarship</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -2951,7 +2947,7 @@
         <v>Chapple/Bremner Scholarship</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -3011,7 +3007,7 @@
         <v>Conservatorium of Music Scholarship</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -3041,7 +3037,7 @@
         <v>Corinna D'Hage Mayer String Scholarship</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -3122,7 +3118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -3143,7 +3139,7 @@
         <v>12</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>162</v>
+        <v>440</v>
       </c>
       <c r="H27" t="s">
         <v>13</v>
@@ -3173,7 +3169,7 @@
         <v>18</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H28" t="s">
         <v>13</v>
@@ -3233,7 +3229,7 @@
         <v>18</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H30" t="s">
         <v>13</v>
@@ -3263,7 +3259,7 @@
         <v>18</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H31" t="s">
         <v>13</v>
@@ -3293,7 +3289,7 @@
         <v>18</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
@@ -3323,7 +3319,7 @@
         <v>18</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H33" t="s">
         <v>13</v>
@@ -3353,7 +3349,7 @@
         <v>18</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H34" t="s">
         <v>13</v>
@@ -3371,7 +3367,7 @@
         <v>Dylis and Milton Renham Scholarship</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -3383,7 +3379,7 @@
         <v>12</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H35" t="s">
         <v>13</v>
@@ -3401,7 +3397,7 @@
         <v>The Donald Lionel Edgerton Scholarship</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -3413,7 +3409,7 @@
         <v>12</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H36" t="s">
         <v>13</v>
@@ -3443,7 +3439,7 @@
         <v>12</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H37" t="s">
         <v>13</v>
@@ -3473,7 +3469,7 @@
         <v>12</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H38" t="s">
         <v>13</v>
@@ -3491,7 +3487,7 @@
         <v>The Elise Herrman Scholarship</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -3503,7 +3499,7 @@
         <v>12</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H39" t="s">
         <v>13</v>
@@ -3533,7 +3529,7 @@
         <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H40" t="s">
         <v>13</v>
@@ -3563,7 +3559,7 @@
         <v>18</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
         <v>13</v>
@@ -3593,7 +3589,7 @@
         <v>18</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H42" t="s">
         <v>13</v>
@@ -3623,7 +3619,7 @@
         <v>12</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H43" t="s">
         <v>13</v>
@@ -3653,7 +3649,7 @@
         <v>12</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H44" t="s">
         <v>13</v>
@@ -3701,7 +3697,7 @@
         <v>Flora Jean Ferriss Scholarship</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D46" t="s">
         <v>14</v>
@@ -3713,7 +3709,7 @@
         <v>12</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H46" t="s">
         <v>13</v>
@@ -3761,7 +3757,7 @@
         <v>Geoffrey Parsons Australian Scholarship</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D48" t="s">
         <v>14</v>
@@ -3773,7 +3769,7 @@
         <v>12</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H48" t="s">
         <v>13</v>
@@ -3791,7 +3787,7 @@
         <v>The Geoffrey Rothwell Scholarship</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D49" t="s">
         <v>14</v>
@@ -3803,7 +3799,7 @@
         <v>12</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H49" t="s">
         <v>13</v>
@@ -3821,7 +3817,7 @@
         <v>George Wallace Henderson Scholarship</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -3833,7 +3829,7 @@
         <v>12</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
@@ -3851,7 +3847,7 @@
         <v>Greenberg-Gurney-Jensen Fund 2</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -3863,7 +3859,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H51" t="s">
         <v>13</v>
@@ -3881,7 +3877,7 @@
         <v>Greenberg-Gurney-Jensen Fund</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D52" t="s">
         <v>14</v>
@@ -3893,7 +3889,7 @@
         <v>12</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H52" t="s">
         <v>13</v>
@@ -3911,7 +3907,7 @@
         <v>Helen Myers Scholarship</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D53" t="s">
         <v>14</v>
@@ -3923,7 +3919,7 @@
         <v>12</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H53" t="s">
         <v>13</v>
@@ -3941,7 +3937,7 @@
         <v>Helen Quach Scholarship</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D54" t="s">
         <v>14</v>
@@ -3953,7 +3949,7 @@
         <v>12</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H54" t="s">
         <v>13</v>
@@ -3983,7 +3979,7 @@
         <v>12</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H55" t="s">
         <v>13</v>
@@ -4001,7 +3997,7 @@
         <v>Henderson Postgraduate Scholarship</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D56" t="s">
         <v>14</v>
@@ -4013,7 +4009,7 @@
         <v>15</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H56" t="s">
         <v>13</v>
@@ -4061,7 +4057,7 @@
         <v>Iremonger Marceau Family Scholarship</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -4073,7 +4069,7 @@
         <v>12</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H58" t="s">
         <v>13</v>
@@ -4103,7 +4099,7 @@
         <v>18</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H59" t="s">
         <v>13</v>
@@ -4133,7 +4129,7 @@
         <v>18</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H60" t="s">
         <v>13</v>
@@ -4163,7 +4159,7 @@
         <v>18</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H61" t="s">
         <v>13</v>
@@ -4181,7 +4177,7 @@
         <v>Jean Giles and Thomas Louis Pidcock Violin Scholarship</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D62" t="s">
         <v>14</v>
@@ -4193,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H62" t="s">
         <v>13</v>
@@ -4211,7 +4207,7 @@
         <v>The Joan and James Armstrong Award</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -4223,7 +4219,7 @@
         <v>12</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H63" t="s">
         <v>13</v>
@@ -4241,7 +4237,7 @@
         <v>John and Dorothy Vimpani Pianoforte Fund</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
@@ -4253,7 +4249,7 @@
         <v>12</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H64" t="s">
         <v>13</v>
@@ -4283,7 +4279,7 @@
         <v>12</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H65" t="s">
         <v>13</v>
@@ -4301,7 +4297,7 @@
         <v>John Luscombe Scholarship for Vocal Studies</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -4313,7 +4309,7 @@
         <v>12</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H66" t="s">
         <v>13</v>
@@ -4343,7 +4339,7 @@
         <v>72</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H67" t="s">
         <v>13</v>
@@ -4373,7 +4369,7 @@
         <v>12</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H68" t="s">
         <v>13</v>
@@ -4391,7 +4387,7 @@
         <v>The Kathleen E Armstrong Bequest</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D69" t="s">
         <v>14</v>
@@ -4403,7 +4399,7 @@
         <v>12</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H69" t="s">
         <v>13</v>
@@ -4421,7 +4417,7 @@
         <v>Keith and Eileen Ong Prize for Piano</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>21</v>
@@ -4451,7 +4447,7 @@
         <v>The Kim Walker Scholarship Endowment Fund</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D71" t="s">
         <v>14</v>
@@ -4463,7 +4459,7 @@
         <v>12</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H71" t="s">
         <v>13</v>
@@ -4481,7 +4477,7 @@
         <v>The Kirkpix Trust Scholarship</v>
       </c>
       <c r="C72" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D72" t="s">
         <v>14</v>
@@ -4493,7 +4489,7 @@
         <v>12</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H72" t="s">
         <v>13</v>
@@ -4571,7 +4567,7 @@
         <v>The Linda Kingsbury Jeffery Scholarship for Singing</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D75" t="s">
         <v>14</v>
@@ -4583,7 +4579,7 @@
         <v>12</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H75" t="s">
         <v>13</v>
@@ -4643,7 +4639,7 @@
         <v>12</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H77" t="s">
         <v>13</v>
@@ -4673,7 +4669,7 @@
         <v>18</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H78" t="s">
         <v>13</v>
@@ -4691,7 +4687,7 @@
         <v>Matteson &amp; Nancy Roberts Violin Scholarship</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
@@ -4703,7 +4699,7 @@
         <v>12</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H79" t="s">
         <v>13</v>
@@ -4751,7 +4747,7 @@
         <v>The Michael Bannigan Scholarship for the Double Bass</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D81" t="s">
         <v>14</v>
@@ -4763,7 +4759,7 @@
         <v>12</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H81" t="s">
         <v>13</v>
@@ -4781,7 +4777,7 @@
         <v>Myron Kantor Bequest</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
@@ -4793,7 +4789,7 @@
         <v>12</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H82" t="s">
         <v>13</v>
@@ -4811,7 +4807,7 @@
         <v>The Olive Margaret Stewart Bequest</v>
       </c>
       <c r="C83" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D83" t="s">
         <v>14</v>
@@ -4823,7 +4819,7 @@
         <v>12</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H83" t="s">
         <v>13</v>
@@ -4841,7 +4837,7 @@
         <v>Orchestra - Witheford Don Scholarship</v>
       </c>
       <c r="C84" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D84" t="s">
         <v>14</v>
@@ -4853,7 +4849,7 @@
         <v>12</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H84" t="s">
         <v>13</v>
@@ -4871,7 +4867,7 @@
         <v>Patricia Bell Grant</v>
       </c>
       <c r="C85" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D85" t="s">
         <v>14</v>
@@ -4883,7 +4879,7 @@
         <v>12</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H85" t="s">
         <v>13</v>
@@ -4913,7 +4909,7 @@
         <v>18</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H86" t="s">
         <v>13</v>
@@ -4943,7 +4939,7 @@
         <v>12</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H87" t="s">
         <v>13</v>
@@ -4973,7 +4969,7 @@
         <v>18</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H88" t="s">
         <v>13</v>
@@ -4991,7 +4987,7 @@
         <v>Peter Davidson Scholarship</v>
       </c>
       <c r="C89" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D89" t="s">
         <v>14</v>
@@ -5003,7 +4999,7 @@
         <v>15</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H89" t="s">
         <v>13</v>
@@ -5081,7 +5077,7 @@
         <v>Queen Victoria Club Scholarship</v>
       </c>
       <c r="C92" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D92" t="s">
         <v>14</v>
@@ -5093,7 +5089,7 @@
         <v>12</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H92" t="s">
         <v>13</v>
@@ -5123,7 +5119,7 @@
         <v>12</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H93" t="s">
         <v>13</v>
@@ -5141,7 +5137,7 @@
         <v>In Memory of Richard Antony Oppen</v>
       </c>
       <c r="C94" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D94" t="s">
         <v>14</v>
@@ -5153,7 +5149,7 @@
         <v>12</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H94" t="s">
         <v>13</v>
@@ -5171,7 +5167,7 @@
         <v>The Richard and Doreen Wilson Organ Scholarship</v>
       </c>
       <c r="C95" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="D95" t="s">
         <v>14</v>
@@ -5183,7 +5179,7 @@
         <v>12</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H95" t="s">
         <v>13</v>
@@ -5201,7 +5197,7 @@
         <v>Richard Merewether French Horn Fellowship</v>
       </c>
       <c r="C96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>14</v>
@@ -5213,7 +5209,7 @@
         <v>12</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H96" t="s">
         <v>13</v>
@@ -5261,7 +5257,7 @@
         <v>The Albert Scholarships</v>
       </c>
       <c r="C98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>30</v>
@@ -5333,7 +5329,7 @@
         <v>12</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H100" t="s">
         <v>13</v>
@@ -5357,13 +5353,13 @@
         <v>6000</v>
       </c>
       <c r="E101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F101" t="s">
         <v>18</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H101" t="s">
         <v>13</v>
@@ -5381,7 +5377,7 @@
         <v>Sarah and Murial Jeavons Memorial Scholarship</v>
       </c>
       <c r="C102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>14</v>
@@ -5393,7 +5389,7 @@
         <v>12</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H102" t="s">
         <v>13</v>
@@ -5423,7 +5419,7 @@
         <v>18</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H103" t="s">
         <v>13</v>
@@ -5471,7 +5467,7 @@
         <v>The Ted and Susan Meller Memorial Scholarship Fund</v>
       </c>
       <c r="C105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>14</v>
@@ -5483,7 +5479,7 @@
         <v>12</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H105" t="s">
         <v>13</v>
@@ -5501,7 +5497,7 @@
         <v>The Chandler Scholarship</v>
       </c>
       <c r="C106" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D106" t="s">
         <v>11</v>
@@ -5513,7 +5509,7 @@
         <v>12</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H106" t="s">
         <v>13</v>
@@ -5531,7 +5527,7 @@
         <v>The Conry Brauer Scholarship for Piano Tuition</v>
       </c>
       <c r="C107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
@@ -5543,7 +5539,7 @@
         <v>12</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H107" t="s">
         <v>13</v>
@@ -5561,7 +5557,7 @@
         <v>The Conry Brauer Scholarship for Violin Tuition</v>
       </c>
       <c r="C108" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>14</v>
@@ -5573,7 +5569,7 @@
         <v>12</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H108" t="s">
         <v>13</v>
@@ -5591,7 +5587,7 @@
         <v>Elizabethan Theatre Trust Ladies’ Committee Scholarship</v>
       </c>
       <c r="C109" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>14</v>
@@ -5603,7 +5599,7 @@
         <v>12</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H109" t="s">
         <v>13</v>
@@ -5621,7 +5617,7 @@
         <v>The Gerald Westheimer Quartet Program</v>
       </c>
       <c r="C110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>14</v>
@@ -5633,7 +5629,7 @@
         <v>12</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H110" t="s">
         <v>13</v>
@@ -5663,7 +5659,7 @@
         <v>18</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H111" t="s">
         <v>13</v>
@@ -5681,7 +5677,7 @@
         <v>The JJ Kelly Memorial Scholarship</v>
       </c>
       <c r="C112" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>11</v>
@@ -5693,7 +5689,7 @@
         <v>12</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H112" t="s">
         <v>13</v>
@@ -5711,7 +5707,7 @@
         <v>The Kevin and Margaret Duffy Scholarship</v>
       </c>
       <c r="C113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>11</v>
@@ -5723,7 +5719,7 @@
         <v>12</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H113" t="s">
         <v>13</v>
@@ -5753,7 +5749,7 @@
         <v>12</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H114" t="s">
         <v>13</v>
@@ -5843,7 +5839,7 @@
         <v>18</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H117" t="s">
         <v>13</v>
@@ -5873,7 +5869,7 @@
         <v>18</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H118" t="s">
         <v>13</v>
@@ -5921,7 +5917,7 @@
         <v>The Vasanta Scholarship</v>
       </c>
       <c r="C120" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>14</v>
@@ -5933,7 +5929,7 @@
         <v>12</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H120" t="s">
         <v>13</v>
@@ -5951,7 +5947,7 @@
         <v>The Verna Florence Dinham Scholarship for Piano</v>
       </c>
       <c r="C121" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>14</v>
@@ -5963,7 +5959,7 @@
         <v>12</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H121" t="s">
         <v>13</v>
@@ -5993,7 +5989,7 @@
         <v>18</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H122" t="s">
         <v>13</v>
@@ -6023,7 +6019,7 @@
         <v>18</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H123" t="s">
         <v>13</v>
@@ -6083,7 +6079,7 @@
         <v>12</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H125" t="s">
         <v>13</v>
@@ -6101,7 +6097,7 @@
         <v>William McIlrath Memorial Scholarship in Music Performance and Research</v>
       </c>
       <c r="C126" t="s">
-        <v>227</v>
+        <v>81</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>14</v>
@@ -6113,7 +6109,7 @@
         <v>15</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H126" t="s">
         <v>13</v>
@@ -6137,13 +6133,13 @@
         <v>10000</v>
       </c>
       <c r="E127" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F127" t="s">
         <v>18</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H127" t="s">
         <v>13</v>
@@ -6173,7 +6169,7 @@
         <v>15</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H128" t="s">
         <v>138</v>
@@ -6203,7 +6199,7 @@
         <v>18</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H129" t="s">
         <v>13</v>
@@ -6233,7 +6229,7 @@
         <v>18</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H130" t="s">
         <v>13</v>
@@ -6263,7 +6259,7 @@
         <v>72</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H131" t="s">
         <v>13</v>
@@ -6293,7 +6289,7 @@
         <v>18</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H132" t="s">
         <v>13</v>
@@ -6323,7 +6319,7 @@
         <v>18</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H133" t="s">
         <v>13</v>
@@ -6353,7 +6349,7 @@
         <v>18</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H134" t="s">
         <v>13</v>
@@ -6383,7 +6379,7 @@
         <v>15</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H135" t="s">
         <v>13</v>
@@ -6413,7 +6409,7 @@
         <v>72</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H136" t="s">
         <v>138</v>
@@ -6443,7 +6439,7 @@
         <v>18</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H137" t="s">
         <v>13</v>
@@ -6473,7 +6469,7 @@
         <v>12</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H138" t="s">
         <v>13</v>
@@ -6533,7 +6529,7 @@
         <v>72</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H140" t="s">
         <v>13</v>
@@ -6563,7 +6559,7 @@
         <v>18</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H141" t="s">
         <v>13</v>
@@ -6593,7 +6589,7 @@
         <v>12</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H142" t="s">
         <v>13</v>
@@ -6623,7 +6619,7 @@
         <v>18</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H143" t="s">
         <v>138</v>
@@ -6683,7 +6679,7 @@
         <v>18</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H145" t="s">
         <v>13</v>
@@ -6713,7 +6709,7 @@
         <v>18</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H146" t="s">
         <v>13</v>
@@ -6737,13 +6733,13 @@
         <v>33</v>
       </c>
       <c r="E147" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F147" t="s">
         <v>18</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H147" t="s">
         <v>13</v>
@@ -6767,13 +6763,13 @@
         <v>21</v>
       </c>
       <c r="E148" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F148" t="s">
         <v>15</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H148" t="s">
         <v>13</v>
@@ -6803,7 +6799,7 @@
         <v>12</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H149" t="s">
         <v>13</v>
@@ -6833,7 +6829,7 @@
         <v>12</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H150" t="s">
         <v>13</v>
@@ -6893,7 +6889,7 @@
         <v>18</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H152" t="s">
         <v>13</v>
@@ -6983,7 +6979,7 @@
         <v>15</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H155" t="s">
         <v>13</v>
@@ -7013,7 +7009,7 @@
         <v>18</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H156" t="s">
         <v>13</v>
@@ -7043,7 +7039,7 @@
         <v>18</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H157" t="s">
         <v>13</v>
@@ -7073,7 +7069,7 @@
         <v>18</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H158" t="s">
         <v>13</v>
@@ -7103,7 +7099,7 @@
         <v>18</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H159" t="s">
         <v>13</v>
@@ -7133,7 +7129,7 @@
         <v>18</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H160" t="s">
         <v>13</v>
@@ -7163,7 +7159,7 @@
         <v>18</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H161" t="s">
         <v>13</v>
@@ -7193,7 +7189,7 @@
         <v>18</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H162" t="s">
         <v>13</v>
@@ -7223,7 +7219,7 @@
         <v>18</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H163" t="s">
         <v>13</v>
@@ -7244,7 +7240,7 @@
         <v>81</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E164" t="s">
         <v>10</v>
@@ -7253,7 +7249,7 @@
         <v>18</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H164" t="s">
         <v>13</v>
@@ -7274,7 +7270,7 @@
         <v>61</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E165" t="s">
         <v>64</v>
@@ -7283,7 +7279,7 @@
         <v>12</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H165" t="s">
         <v>13</v>
@@ -7313,7 +7309,7 @@
         <v>18</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H166" t="s">
         <v>13</v>
@@ -7343,7 +7339,7 @@
         <v>15</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H167" t="s">
         <v>13</v>
@@ -7373,7 +7369,7 @@
         <v>18</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H168" t="s">
         <v>13</v>
@@ -7403,7 +7399,7 @@
         <v>18</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H169" t="s">
         <v>13</v>
@@ -7427,13 +7423,13 @@
         <v>22</v>
       </c>
       <c r="E170" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F170" t="s">
         <v>15</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H170" t="s">
         <v>13</v>
@@ -7463,7 +7459,7 @@
         <v>18</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H171" t="s">
         <v>13</v>
@@ -7493,7 +7489,7 @@
         <v>18</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H172" t="s">
         <v>13</v>
@@ -7523,7 +7519,7 @@
         <v>72</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H173" t="s">
         <v>13</v>
@@ -7553,7 +7549,7 @@
         <v>15</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H174" t="s">
         <v>13</v>
@@ -7577,13 +7573,13 @@
         <v>41</v>
       </c>
       <c r="E175" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F175" t="s">
         <v>18</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H175" t="s">
         <v>13</v>
@@ -7613,7 +7609,7 @@
         <v>12</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H176" t="s">
         <v>13</v>
@@ -7643,7 +7639,7 @@
         <v>12</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H177" t="s">
         <v>13</v>
@@ -7673,7 +7669,7 @@
         <v>18</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H178" t="s">
         <v>13</v>
@@ -7703,7 +7699,7 @@
         <v>15</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H179" t="s">
         <v>13</v>
@@ -7733,7 +7729,7 @@
         <v>18</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H180" t="s">
         <v>13</v>
@@ -7763,7 +7759,7 @@
         <v>18</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H181" t="s">
         <v>13</v>
@@ -7793,7 +7789,7 @@
         <v>12</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H182" t="s">
         <v>13</v>
@@ -7823,7 +7819,7 @@
         <v>18</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H183" t="s">
         <v>13</v>
@@ -7853,7 +7849,7 @@
         <v>15</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H184" t="s">
         <v>13</v>
@@ -7883,7 +7879,7 @@
         <v>18</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H185" t="s">
         <v>13</v>
@@ -7913,7 +7909,7 @@
         <v>18</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H186" t="s">
         <v>13</v>
@@ -7943,7 +7939,7 @@
         <v>18</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H187" t="s">
         <v>13</v>
@@ -8003,7 +7999,7 @@
         <v>18</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H189" t="s">
         <v>13</v>
@@ -8033,7 +8029,7 @@
         <v>12</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H190" t="s">
         <v>13</v>
@@ -8063,7 +8059,7 @@
         <v>18</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H191" t="s">
         <v>13</v>
@@ -8093,7 +8089,7 @@
         <v>18</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H192" t="s">
         <v>13</v>
@@ -8123,7 +8119,7 @@
         <v>15</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H193" t="s">
         <v>13</v>
@@ -8144,7 +8140,7 @@
         <v>81</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E194" t="s">
         <v>10</v>
@@ -8153,7 +8149,7 @@
         <v>18</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H194" t="s">
         <v>138</v>
@@ -8174,7 +8170,7 @@
         <v>61</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E195" t="s">
         <v>10</v>
@@ -8183,7 +8179,7 @@
         <v>18</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H195" t="s">
         <v>13</v>
@@ -8213,7 +8209,7 @@
         <v>15</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H196" t="s">
         <v>13</v>
@@ -8243,7 +8239,7 @@
         <v>12</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H197" t="s">
         <v>13</v>
@@ -8273,7 +8269,7 @@
         <v>18</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H198" t="s">
         <v>13</v>
@@ -8303,7 +8299,7 @@
         <v>18</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H199" t="s">
         <v>13</v>
@@ -8333,7 +8329,7 @@
         <v>12</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H200" t="s">
         <v>13</v>
@@ -8363,7 +8359,7 @@
         <v>12</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H201" t="s">
         <v>13</v>
@@ -8393,7 +8389,7 @@
         <v>15</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H202" t="s">
         <v>13</v>
@@ -8423,7 +8419,7 @@
         <v>12</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H203" t="s">
         <v>13</v>
@@ -8453,7 +8449,7 @@
         <v>18</v>
       </c>
       <c r="G204" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H204" t="s">
         <v>13</v>
@@ -8483,7 +8479,7 @@
         <v>15</v>
       </c>
       <c r="G205" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H205" t="s">
         <v>13</v>
@@ -8513,7 +8509,7 @@
         <v>15</v>
       </c>
       <c r="G206" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H206" t="s">
         <v>13</v>
@@ -8543,7 +8539,7 @@
         <v>18</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H207" t="s">
         <v>13</v>
@@ -8573,7 +8569,7 @@
         <v>18</v>
       </c>
       <c r="G208" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H208" t="s">
         <v>13</v>
@@ -8594,7 +8590,7 @@
         <v>61</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E209" t="s">
         <v>64</v>
@@ -8603,7 +8599,7 @@
         <v>12</v>
       </c>
       <c r="G209" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H209" t="s">
         <v>13</v>
@@ -8633,7 +8629,7 @@
         <v>18</v>
       </c>
       <c r="G210" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H210" t="s">
         <v>138</v>
@@ -8663,7 +8659,7 @@
         <v>18</v>
       </c>
       <c r="G211" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H211" t="s">
         <v>13</v>
@@ -8693,7 +8689,7 @@
         <v>72</v>
       </c>
       <c r="G212" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H212" t="s">
         <v>13</v>
@@ -8717,13 +8713,13 @@
         <v>22</v>
       </c>
       <c r="E213" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F213" t="s">
         <v>18</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H213" t="s">
         <v>13</v>
@@ -8753,7 +8749,7 @@
         <v>15</v>
       </c>
       <c r="G214" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H214" t="s">
         <v>13</v>
@@ -8813,7 +8809,7 @@
         <v>15</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H216" t="s">
         <v>13</v>
@@ -8831,7 +8827,7 @@
         <v>Sydney Symposium Choral Foundation Conducting Scholarship</v>
       </c>
       <c r="C217" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D217" t="s">
         <v>14</v>
@@ -8843,7 +8839,7 @@
         <v>12</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H217" t="s">
         <v>13</v>
@@ -8903,7 +8899,7 @@
         <v>12</v>
       </c>
       <c r="G219" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H219" t="s">
         <v>13</v>
@@ -8933,7 +8929,7 @@
         <v>12</v>
       </c>
       <c r="G220" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H220" t="s">
         <v>13</v>
@@ -8963,7 +8959,7 @@
         <v>12</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H221" t="s">
         <v>13</v>
@@ -8993,7 +8989,7 @@
         <v>18</v>
       </c>
       <c r="G222" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H222" t="s">
         <v>13</v>
@@ -9023,7 +9019,7 @@
         <v>18</v>
       </c>
       <c r="G223" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H223" t="s">
         <v>13</v>
@@ -9053,7 +9049,7 @@
         <v>18</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H224" t="s">
         <v>13</v>
@@ -9083,7 +9079,7 @@
         <v>72</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H225" t="s">
         <v>13</v>
@@ -9113,7 +9109,7 @@
         <v>18</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H226" t="s">
         <v>13</v>
@@ -9143,7 +9139,7 @@
         <v>12</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H227" t="s">
         <v>13</v>
@@ -9173,7 +9169,7 @@
         <v>12</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H228" t="s">
         <v>13</v>
@@ -9203,7 +9199,7 @@
         <v>15</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H229" t="s">
         <v>13</v>
@@ -9227,13 +9223,13 @@
         <v>28</v>
       </c>
       <c r="E230" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F230" t="s">
         <v>15</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H230" t="s">
         <v>13</v>
@@ -9263,7 +9259,7 @@
         <v>18</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H231" t="s">
         <v>13</v>
@@ -9287,13 +9283,13 @@
         <v>20000</v>
       </c>
       <c r="E232" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F232" t="s">
         <v>18</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H232" t="s">
         <v>13</v>
@@ -9323,7 +9319,7 @@
         <v>12</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H233" t="s">
         <v>13</v>
@@ -9353,7 +9349,7 @@
         <v>12</v>
       </c>
       <c r="G234" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H234" t="s">
         <v>13</v>
@@ -9383,7 +9379,7 @@
         <v>18</v>
       </c>
       <c r="G235" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H235" t="s">
         <v>13</v>
@@ -9413,7 +9409,7 @@
         <v>10</v>
       </c>
       <c r="G236" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H236" t="s">
         <v>13</v>
@@ -9443,7 +9439,7 @@
         <v>18</v>
       </c>
       <c r="G237" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H237" t="s">
         <v>13</v>
@@ -9473,7 +9469,7 @@
         <v>18</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H238" t="s">
         <v>13</v>
@@ -9503,7 +9499,7 @@
         <v>18</v>
       </c>
       <c r="G239" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H239" t="s">
         <v>13</v>
@@ -9563,7 +9559,7 @@
         <v>18</v>
       </c>
       <c r="G241" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H241" t="s">
         <v>13</v>
@@ -9593,7 +9589,7 @@
         <v>18</v>
       </c>
       <c r="G242" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H242" t="s">
         <v>13</v>
@@ -9653,7 +9649,7 @@
         <v>15</v>
       </c>
       <c r="G244" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H244" t="s">
         <v>13</v>
@@ -9683,7 +9679,7 @@
         <v>18</v>
       </c>
       <c r="G245" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H245" t="s">
         <v>138</v>
@@ -9713,7 +9709,7 @@
         <v>12</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H246" t="s">
         <v>13</v>
@@ -9803,7 +9799,7 @@
         <v>12</v>
       </c>
       <c r="G249" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H249" t="s">
         <v>13</v>
@@ -9824,7 +9820,7 @@
         <v>61</v>
       </c>
       <c r="D250" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E250" t="s">
         <v>10</v>
@@ -9833,7 +9829,7 @@
         <v>15</v>
       </c>
       <c r="G250" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H250" t="s">
         <v>13</v>
@@ -9893,7 +9889,7 @@
         <v>10</v>
       </c>
       <c r="G252" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H252" t="s">
         <v>13</v>
@@ -9923,7 +9919,7 @@
         <v>12</v>
       </c>
       <c r="G253" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H253" t="s">
         <v>13</v>
@@ -9953,7 +9949,7 @@
         <v>12</v>
       </c>
       <c r="G254" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H254" t="s">
         <v>13</v>
@@ -9983,7 +9979,7 @@
         <v>12</v>
       </c>
       <c r="G255" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H255" t="s">
         <v>13</v>
@@ -10007,13 +10003,13 @@
         <v>22</v>
       </c>
       <c r="E256" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F256" t="s">
         <v>15</v>
       </c>
       <c r="G256" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H256" t="s">
         <v>13</v>
@@ -10037,13 +10033,13 @@
         <v>22</v>
       </c>
       <c r="E257" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F257" t="s">
         <v>15</v>
       </c>
       <c r="G257" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H257" t="s">
         <v>13</v>
@@ -10067,13 +10063,13 @@
         <v>22</v>
       </c>
       <c r="E258" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F258" t="s">
         <v>15</v>
       </c>
       <c r="G258" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H258" t="s">
         <v>13</v>
@@ -10103,7 +10099,7 @@
         <v>10</v>
       </c>
       <c r="G259" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H259" t="s">
         <v>13</v>
@@ -10133,7 +10129,7 @@
         <v>12</v>
       </c>
       <c r="G260" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H260" t="s">
         <v>138</v>
@@ -10163,7 +10159,7 @@
         <v>18</v>
       </c>
       <c r="G261" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H261" t="s">
         <v>13</v>
@@ -10193,7 +10189,7 @@
         <v>10</v>
       </c>
       <c r="G262" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H262" t="s">
         <v>13</v>
@@ -10217,13 +10213,13 @@
         <v>22</v>
       </c>
       <c r="E263" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F263" t="s">
         <v>15</v>
       </c>
       <c r="G263" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H263" t="s">
         <v>13</v>
@@ -10247,13 +10243,13 @@
         <v>22</v>
       </c>
       <c r="E264" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F264" t="s">
         <v>15</v>
       </c>
       <c r="G264" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H264" t="s">
         <v>13</v>
@@ -10277,13 +10273,13 @@
         <v>22</v>
       </c>
       <c r="E265" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F265" t="s">
         <v>15</v>
       </c>
       <c r="G265" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H265" t="s">
         <v>13</v>
@@ -10337,13 +10333,13 @@
         <v>8625</v>
       </c>
       <c r="E267" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F267" t="s">
         <v>15</v>
       </c>
       <c r="G267" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H267" t="s">
         <v>13</v>
@@ -10367,13 +10363,13 @@
         <v>24</v>
       </c>
       <c r="E268" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F268" t="s">
+        <v>18</v>
+      </c>
+      <c r="G268" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="F268" t="s">
-        <v>18</v>
-      </c>
-      <c r="G268" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="H268" t="s">
         <v>13</v>
@@ -10397,13 +10393,13 @@
         <v>52</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F269" t="s">
         <v>15</v>
       </c>
       <c r="G269" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H269" t="s">
         <v>13</v>
@@ -10433,7 +10429,7 @@
         <v>18</v>
       </c>
       <c r="G270" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H270" t="s">
         <v>13</v>
@@ -10463,7 +10459,7 @@
         <v>15</v>
       </c>
       <c r="G271" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H271" t="s">
         <v>13</v>
@@ -10493,7 +10489,7 @@
         <v>15</v>
       </c>
       <c r="G272" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H272" t="s">
         <v>13</v>
@@ -10514,16 +10510,16 @@
         <v>61</v>
       </c>
       <c r="D273" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E273" t="s">
         <v>367</v>
-      </c>
-      <c r="E273" t="s">
-        <v>368</v>
       </c>
       <c r="F273" t="s">
         <v>15</v>
       </c>
       <c r="G273" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H273" t="s">
         <v>13</v>
@@ -10553,7 +10549,7 @@
         <v>18</v>
       </c>
       <c r="G274" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H274" t="s">
         <v>13</v>
@@ -10583,7 +10579,7 @@
         <v>18</v>
       </c>
       <c r="G275" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H275" t="s">
         <v>13</v>
@@ -10613,7 +10609,7 @@
         <v>15</v>
       </c>
       <c r="G276" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H276" t="s">
         <v>13</v>
@@ -10673,7 +10669,7 @@
         <v>15</v>
       </c>
       <c r="G278" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H278" t="s">
         <v>13</v>
@@ -10697,13 +10693,13 @@
         <v>5000</v>
       </c>
       <c r="E279" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F279" t="s">
         <v>15</v>
       </c>
       <c r="G279" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H279" t="s">
         <v>13</v>
@@ -10733,7 +10729,7 @@
         <v>18</v>
       </c>
       <c r="G280" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H280" t="s">
         <v>13</v>
@@ -10763,7 +10759,7 @@
         <v>15</v>
       </c>
       <c r="G281" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H281" t="s">
         <v>13</v>
@@ -10793,7 +10789,7 @@
         <v>18</v>
       </c>
       <c r="G282" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H282" t="s">
         <v>13</v>
@@ -10853,7 +10849,7 @@
         <v>15</v>
       </c>
       <c r="G284" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H284" t="s">
         <v>138</v>
@@ -10883,7 +10879,7 @@
         <v>18</v>
       </c>
       <c r="G285" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H285" t="s">
         <v>13</v>
@@ -10907,13 +10903,13 @@
         <v>25000</v>
       </c>
       <c r="E286" t="s">
+        <v>378</v>
+      </c>
+      <c r="F286" t="s">
+        <v>18</v>
+      </c>
+      <c r="G286" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="F286" t="s">
-        <v>18</v>
-      </c>
-      <c r="G286" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="H286" t="s">
         <v>13</v>
@@ -10943,7 +10939,7 @@
         <v>18</v>
       </c>
       <c r="G287" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H287" t="s">
         <v>13</v>
@@ -10973,7 +10969,7 @@
         <v>18</v>
       </c>
       <c r="G288" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H288" t="s">
         <v>13</v>
@@ -11003,7 +10999,7 @@
         <v>15</v>
       </c>
       <c r="G289" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H289" t="s">
         <v>13</v>
@@ -11033,7 +11029,7 @@
         <v>15</v>
       </c>
       <c r="G290" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H290" t="s">
         <v>13</v>
@@ -11057,13 +11053,13 @@
         <v>19</v>
       </c>
       <c r="E291" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F291" t="s">
         <v>18</v>
       </c>
       <c r="G291" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H291" t="s">
         <v>13</v>
@@ -11123,7 +11119,7 @@
         <v>18</v>
       </c>
       <c r="G293" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H293" t="s">
         <v>13</v>
@@ -11153,7 +11149,7 @@
         <v>18</v>
       </c>
       <c r="G294" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H294" t="s">
         <v>13</v>
@@ -11183,7 +11179,7 @@
         <v>15</v>
       </c>
       <c r="G295" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H295" t="s">
         <v>13</v>
@@ -11207,13 +11203,13 @@
         <v>32</v>
       </c>
       <c r="E296" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F296" t="s">
         <v>18</v>
       </c>
       <c r="G296" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H296" t="s">
         <v>13</v>
@@ -11243,7 +11239,7 @@
         <v>18</v>
       </c>
       <c r="G297" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H297" t="s">
         <v>13</v>
@@ -11273,7 +11269,7 @@
         <v>18</v>
       </c>
       <c r="G298" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H298" t="s">
         <v>13</v>
@@ -11303,7 +11299,7 @@
         <v>18</v>
       </c>
       <c r="G299" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H299" t="s">
         <v>13</v>
@@ -11333,7 +11329,7 @@
         <v>18</v>
       </c>
       <c r="G300" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H300" t="s">
         <v>13</v>
@@ -11363,7 +11359,7 @@
         <v>18</v>
       </c>
       <c r="G301" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H301" t="s">
         <v>13</v>
@@ -11393,7 +11389,7 @@
         <v>72</v>
       </c>
       <c r="G302" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H302" t="s">
         <v>13</v>
@@ -11423,7 +11419,7 @@
         <v>15</v>
       </c>
       <c r="G303" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H303" t="s">
         <v>13</v>
@@ -11453,7 +11449,7 @@
         <v>18</v>
       </c>
       <c r="G304" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H304" t="s">
         <v>13</v>
@@ -11513,7 +11509,7 @@
         <v>12</v>
       </c>
       <c r="G306" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H306" t="s">
         <v>13</v>
@@ -11537,13 +11533,13 @@
         <v>26</v>
       </c>
       <c r="E307" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F307" t="s">
         <v>18</v>
       </c>
       <c r="G307" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H307" t="s">
         <v>13</v>
@@ -11573,7 +11569,7 @@
         <v>18</v>
       </c>
       <c r="G308" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H308" t="s">
         <v>13</v>
@@ -11603,7 +11599,7 @@
         <v>72</v>
       </c>
       <c r="G309" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H309" t="s">
         <v>13</v>
@@ -11633,7 +11629,7 @@
         <v>72</v>
       </c>
       <c r="G310" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H310" t="s">
         <v>13</v>
@@ -11663,7 +11659,7 @@
         <v>15</v>
       </c>
       <c r="G311" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H311" t="s">
         <v>13</v>
@@ -11693,7 +11689,7 @@
         <v>15</v>
       </c>
       <c r="G312" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H312" t="s">
         <v>13</v>
@@ -11723,7 +11719,7 @@
         <v>18</v>
       </c>
       <c r="G313" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H313" t="s">
         <v>13</v>
@@ -11753,7 +11749,7 @@
         <v>15</v>
       </c>
       <c r="G314" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H314" t="s">
         <v>13</v>
@@ -11783,7 +11779,7 @@
         <v>18</v>
       </c>
       <c r="G315" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H315" t="s">
         <v>13</v>
@@ -11813,7 +11809,7 @@
         <v>18</v>
       </c>
       <c r="G316" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H316" t="s">
         <v>13</v>
@@ -11873,7 +11869,7 @@
         <v>18</v>
       </c>
       <c r="G318" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H318" t="s">
         <v>13</v>
@@ -11903,7 +11899,7 @@
         <v>15</v>
       </c>
       <c r="G319" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H319" t="s">
         <v>13</v>
@@ -11993,7 +11989,7 @@
         <v>18</v>
       </c>
       <c r="G322" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H322" t="s">
         <v>13</v>
@@ -12023,7 +12019,7 @@
         <v>18</v>
       </c>
       <c r="G323" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H323" t="s">
         <v>13</v>
@@ -12053,7 +12049,7 @@
         <v>15</v>
       </c>
       <c r="G324" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H324" t="s">
         <v>13</v>
@@ -12083,7 +12079,7 @@
         <v>18</v>
       </c>
       <c r="G325" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H325" t="s">
         <v>13</v>
@@ -12113,7 +12109,7 @@
         <v>15</v>
       </c>
       <c r="G326" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H326" t="s">
         <v>13</v>
@@ -12143,7 +12139,7 @@
         <v>72</v>
       </c>
       <c r="G327" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H327" t="s">
         <v>13</v>
@@ -12173,7 +12169,7 @@
         <v>18</v>
       </c>
       <c r="G328" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H328" t="s">
         <v>13</v>
@@ -12197,13 +12193,13 @@
         <v>24</v>
       </c>
       <c r="E329" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F329" t="s">
+        <v>18</v>
+      </c>
+      <c r="G329" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F329" t="s">
-        <v>18</v>
-      </c>
-      <c r="G329" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="H329" t="s">
         <v>13</v>
@@ -12233,7 +12229,7 @@
         <v>18</v>
       </c>
       <c r="G330" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H330" t="s">
         <v>13</v>
@@ -12257,13 +12253,13 @@
         <v>21</v>
       </c>
       <c r="E331" t="s">
+        <v>418</v>
+      </c>
+      <c r="F331" t="s">
+        <v>18</v>
+      </c>
+      <c r="G331" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="F331" t="s">
-        <v>18</v>
-      </c>
-      <c r="G331" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="H331" t="s">
         <v>13</v>
@@ -12293,7 +12289,7 @@
         <v>18</v>
       </c>
       <c r="G332" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H332" t="s">
         <v>13</v>
@@ -12380,10 +12376,10 @@
         <v>64</v>
       </c>
       <c r="F335" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G335" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H335" t="s">
         <v>13</v>
@@ -12413,7 +12409,7 @@
         <v>18</v>
       </c>
       <c r="G336" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H336" t="s">
         <v>13</v>
@@ -12443,7 +12439,7 @@
         <v>18</v>
       </c>
       <c r="G337" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H337" t="s">
         <v>13</v>
@@ -12473,7 +12469,7 @@
         <v>18</v>
       </c>
       <c r="G338" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H338" t="s">
         <v>13</v>
@@ -12533,7 +12529,7 @@
         <v>18</v>
       </c>
       <c r="G340" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H340" t="s">
         <v>13</v>
@@ -12563,7 +12559,7 @@
         <v>18</v>
       </c>
       <c r="G341" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H341" t="s">
         <v>13</v>
@@ -12587,13 +12583,13 @@
         <v>31</v>
       </c>
       <c r="E342" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F342" t="s">
         <v>15</v>
       </c>
       <c r="G342" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H342" t="s">
         <v>13</v>
@@ -12623,7 +12619,7 @@
         <v>18</v>
       </c>
       <c r="G343" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H343" t="s">
         <v>13</v>
@@ -12653,7 +12649,7 @@
         <v>18</v>
       </c>
       <c r="G344" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H344" t="s">
         <v>13</v>
@@ -12683,7 +12679,7 @@
         <v>12</v>
       </c>
       <c r="G345" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H345" t="s">
         <v>13</v>
@@ -12699,6 +12695,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1B59F058DD61F4CBF5D961017DC0A45" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3843482ad259dd7cf47d53181de3a479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="514dc54e-a510-4ebc-96a4-7a373c84d576" xmlns:ns3="91d47d42-378c-4240-adf1-50612b639f36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2a99e4d2b0f67119e90f9a433f5d6db" ns2:_="" ns3:_="">
     <xsd:import namespace="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
@@ -12947,27 +12963,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="514dc54e-a510-4ebc-96a4-7a373c84d576">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="91d47d42-378c-4240-adf1-50612b639f36" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985306DE-D9ED-4910-9266-5518F73180B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A196ED53-76B1-4E3A-A1A0-FAA4CB69303D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
+    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FCA4502-B782-48B7-9C63-396C70029E53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12984,23 +12999,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A196ED53-76B1-4E3A-A1A0-FAA4CB69303D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="514dc54e-a510-4ebc-96a4-7a373c84d576"/>
-    <ds:schemaRef ds:uri="91d47d42-378c-4240-adf1-50612b639f36"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985306DE-D9ED-4910-9266-5518F73180B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>